<commit_message>
inicia insercao da tipologia de alteracoes gsim
</commit_message>
<xml_diff>
--- a/20230525T135146/execucao.xlsx
+++ b/20230525T135146/execucao.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fjunior/Projects/notas/20230525T135146/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fjunior/Projects/splor/notas/20230525T135146/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E54C1BF-69C0-814C-B8EC-88C36F9335EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFBF14A0-6CD4-E548-8475-1ADBA97F38EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16240" yWindow="500" windowWidth="19200" windowHeight="21100" xr2:uid="{61A20376-4272-3E43-82F5-99DB9507BC97}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{61A20376-4272-3E43-82F5-99DB9507BC97}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="24">
   <si>
     <t>doc</t>
   </si>
@@ -102,6 +103,12 @@
   </si>
   <si>
     <t>FHEMIG não voltou para a fonte 60</t>
+  </si>
+  <si>
+    <t>uo_cod</t>
+  </si>
+  <si>
+    <t>uo_sigla</t>
   </si>
 </sst>
 </file>
@@ -468,12 +475,326 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC20CFDE-9849-4445-ACE4-CC0A7DB38B47}">
-  <dimension ref="A1:H16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B73A6EEE-2768-924F-810F-C43631938AEA}">
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection sqref="A1:G16"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="22.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2009</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2010</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2011</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="2"/>
+      <c r="B2">
+        <v>9901</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="2">
+        <v>50</v>
+      </c>
+      <c r="G2" s="2">
+        <v>50</v>
+      </c>
+      <c r="H2" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="2"/>
+      <c r="B3">
+        <v>9901</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="2">
+        <v>25</v>
+      </c>
+      <c r="G3" s="2">
+        <v>25</v>
+      </c>
+      <c r="H3" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="2"/>
+      <c r="B4">
+        <v>2301</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="2">
+        <v>15</v>
+      </c>
+      <c r="G4" s="2">
+        <v>15</v>
+      </c>
+      <c r="H4" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="2"/>
+      <c r="B5">
+        <v>1251</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5">
+        <v>60</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="2">
+        <v>10</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="2"/>
+      <c r="B6">
+        <v>1251</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
+        <v>10</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="2"/>
+      <c r="B7">
+        <v>2271</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7">
+        <v>60</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="2">
+        <v>5</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="2"/>
+      <c r="B8">
+        <v>2271</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8">
+        <v>20</v>
+      </c>
+      <c r="E8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2">
+        <v>5</v>
+      </c>
+      <c r="H8" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="2"/>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18">
+        <v>10</v>
+      </c>
+      <c r="E18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19">
+        <v>20</v>
+      </c>
+      <c r="E19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20">
+        <v>20</v>
+      </c>
+      <c r="E20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21">
+        <v>60</v>
+      </c>
+      <c r="E21" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" s="2">
+        <v>10</v>
+      </c>
+      <c r="G21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22">
+        <v>20</v>
+      </c>
+      <c r="E22" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" s="2">
+        <v>5</v>
+      </c>
+      <c r="G22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC20CFDE-9849-4445-ACE4-CC0A7DB38B47}">
+  <dimension ref="A1:J16"/>
+  <sheetViews>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -481,7 +802,7 @@
     <col min="8" max="8" width="30.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -506,8 +827,14 @@
       <c r="H1" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1">
+        <v>2009</v>
+      </c>
+      <c r="J1">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -530,7 +857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -553,7 +880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -576,7 +903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -599,7 +926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -622,7 +949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -645,7 +972,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -668,7 +995,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -691,7 +1018,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -717,7 +1044,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -743,7 +1070,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -766,7 +1093,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -789,7 +1116,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -812,7 +1139,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -838,7 +1165,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
altera para eventos reais das fontes de recurso
</commit_message>
<xml_diff>
--- a/20230525T135146/execucao.xlsx
+++ b/20230525T135146/execucao.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fjunior/Projects/splor/notas/20230525T135146/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFBF14A0-6CD4-E548-8475-1ADBA97F38EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6919B25-D359-7348-9D7F-197A1B070A9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{61A20376-4272-3E43-82F5-99DB9507BC97}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="wide" sheetId="2" r:id="rId1"/>
+    <sheet name="long" sheetId="1" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">wide!$A$1:$W$14</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="21" r:id="rId3"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="34">
   <si>
     <t>doc</t>
   </si>
@@ -109,14 +115,45 @@
   </si>
   <si>
     <t>uo_sigla</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Sum of 2002</t>
+  </si>
+  <si>
+    <t>Sum of 2003</t>
+  </si>
+  <si>
+    <t>Sum of 2004</t>
+  </si>
+  <si>
+    <t>SES</t>
+  </si>
+  <si>
+    <t>Sum of 2005</t>
+  </si>
+  <si>
+    <t>Sum of 2006</t>
+  </si>
+  <si>
+    <t>Sum of 2007</t>
+  </si>
+  <si>
+    <t>Taxa florestal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -155,12 +192,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -177,6 +220,339 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Francisco Junior" refreshedDate="45093.395998842592" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="11" xr:uid="{7DA3154A-A7B2-8949-8C70-24ECAB55D884}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:N14" sheet="wide"/>
+  </cacheSource>
+  <cacheFields count="14">
+    <cacheField name="uo_cod" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1251" maxValue="9901"/>
+    </cacheField>
+    <cacheField name="uo_sigla" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="cod" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="10" maxValue="61" count="4">
+        <n v="10"/>
+        <n v="20"/>
+        <n v="60"/>
+        <n v="61"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="hist" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="2002" numFmtId="164">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="50"/>
+    </cacheField>
+    <cacheField name="2003" numFmtId="164">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="50"/>
+    </cacheField>
+    <cacheField name="2004" numFmtId="164">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="50"/>
+    </cacheField>
+    <cacheField name="2005" numFmtId="164">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="50"/>
+    </cacheField>
+    <cacheField name="2006" numFmtId="164">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="50"/>
+    </cacheField>
+    <cacheField name="2007" numFmtId="164">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="50"/>
+    </cacheField>
+    <cacheField name="2008" numFmtId="164">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="2009" numFmtId="164">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="0" maxValue="50"/>
+    </cacheField>
+    <cacheField name="2010" numFmtId="164">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="0" maxValue="50"/>
+    </cacheField>
+    <cacheField name="2011" numFmtId="164">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="0" maxValue="50"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="11">
+  <r>
+    <n v="9901"/>
+    <s v="TESOURO"/>
+    <x v="0"/>
+    <s v="ICMS"/>
+    <n v="50"/>
+    <n v="50"/>
+    <n v="50"/>
+    <n v="50"/>
+    <n v="50"/>
+    <n v="50"/>
+    <m/>
+    <n v="50"/>
+    <n v="50"/>
+    <n v="50"/>
+  </r>
+  <r>
+    <n v="9901"/>
+    <s v="TESOURO"/>
+    <x v="1"/>
+    <s v="Taxa de segurança pública"/>
+    <n v="25"/>
+    <n v="25"/>
+    <n v="25"/>
+    <n v="25"/>
+    <n v="25"/>
+    <n v="25"/>
+    <m/>
+    <n v="25"/>
+    <n v="25"/>
+    <n v="25"/>
+  </r>
+  <r>
+    <n v="2301"/>
+    <s v="DER"/>
+    <x v="1"/>
+    <s v="CIDE"/>
+    <n v="15"/>
+    <n v="15"/>
+    <n v="15"/>
+    <n v="15"/>
+    <n v="15"/>
+    <n v="15"/>
+    <m/>
+    <n v="15"/>
+    <n v="15"/>
+    <n v="15"/>
+  </r>
+  <r>
+    <n v="1251"/>
+    <s v="PMMG"/>
+    <x v="2"/>
+    <s v="Concursos"/>
+    <n v="10"/>
+    <n v="10"/>
+    <n v="0"/>
+    <n v="10"/>
+    <n v="10"/>
+    <n v="10"/>
+    <m/>
+    <n v="10"/>
+    <n v="0"/>
+    <n v="10"/>
+  </r>
+  <r>
+    <n v="1251"/>
+    <s v="PMMG"/>
+    <x v="0"/>
+    <s v="Concursos"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="10"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <m/>
+    <n v="0"/>
+    <n v="10"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="1321"/>
+    <s v="SES"/>
+    <x v="2"/>
+    <s v="SUS"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="0"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <n v="1321"/>
+    <s v="SES"/>
+    <x v="3"/>
+    <s v="SUS"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="5"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <n v="1321"/>
+    <s v="SES"/>
+    <x v="1"/>
+    <s v="SUS"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="5"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <n v="2271"/>
+    <s v="FHEMIG"/>
+    <x v="2"/>
+    <s v="SUS"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <m/>
+    <n v="5"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="2271"/>
+    <s v="FHEMIG"/>
+    <x v="1"/>
+    <s v="SUS"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="0"/>
+    <m/>
+    <n v="0"/>
+    <n v="5"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <n v="2271"/>
+    <s v="FHEMIG"/>
+    <x v="3"/>
+    <s v="SUS"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="5"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F0259708-AAAD-D74F-BF6E-82E1608099B0}" name="PivotTable1" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="Q16:W21" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="14">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" numFmtId="164" showAll="0"/>
+    <pivotField dataField="1" numFmtId="164" showAll="0"/>
+    <pivotField dataField="1" numFmtId="164" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+    <i i="3">
+      <x v="3"/>
+    </i>
+    <i i="4">
+      <x v="4"/>
+    </i>
+    <i i="5">
+      <x v="5"/>
+    </i>
+  </colItems>
+  <dataFields count="6">
+    <dataField name="Sum of 2002" fld="4" baseField="0" baseItem="0"/>
+    <dataField name="Sum of 2003" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of 2004" fld="6" baseField="0" baseItem="0"/>
+    <dataField name="Sum of 2005" fld="7" baseField="0" baseItem="0"/>
+    <dataField name="Sum of 2006" fld="8" baseField="0" baseItem="0"/>
+    <dataField name="Sum of 2007" fld="9" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -476,314 +852,795 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B73A6EEE-2768-924F-810F-C43631938AEA}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:W28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="11" width="6" customWidth="1"/>
+    <col min="12" max="14" width="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="2.83203125" customWidth="1"/>
+    <col min="17" max="17" width="13" bestFit="1" customWidth="1"/>
+    <col min="18" max="23" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1">
+        <v>2002</v>
+      </c>
       <c r="F1" s="1">
+        <v>2003</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2004</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2005</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2006</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2007</v>
+      </c>
+      <c r="K1" s="1">
+        <v>2008</v>
+      </c>
+      <c r="L1" s="1">
         <v>2009</v>
       </c>
-      <c r="G1" s="1">
+      <c r="M1" s="1">
         <v>2010</v>
       </c>
-      <c r="H1" s="1">
+      <c r="N1" s="1">
         <v>2011</v>
       </c>
-      <c r="I1" s="1">
+      <c r="O1" s="1">
         <v>2012</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="2"/>
-      <c r="B2">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A2">
         <v>9901</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="D2">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="2">
+      <c r="E2" s="3">
         <v>50</v>
       </c>
-      <c r="G2" s="2">
+      <c r="F2" s="3">
         <v>50</v>
       </c>
-      <c r="H2" s="2">
+      <c r="G2" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
-      <c r="B3">
+      <c r="H2" s="3">
+        <v>50</v>
+      </c>
+      <c r="I2" s="3">
+        <v>50</v>
+      </c>
+      <c r="J2" s="3">
+        <v>50</v>
+      </c>
+      <c r="K2" s="3">
+        <v>50</v>
+      </c>
+      <c r="L2" s="3">
+        <v>50</v>
+      </c>
+      <c r="M2" s="3">
+        <v>50</v>
+      </c>
+      <c r="N2" s="3">
+        <v>50</v>
+      </c>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A3">
         <v>9901</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="D3">
+      <c r="C3">
+        <v>59</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="3">
+        <v>25</v>
+      </c>
+      <c r="F3" s="3">
+        <v>25</v>
+      </c>
+      <c r="G3" s="3">
+        <v>25</v>
+      </c>
+      <c r="H3" s="3">
+        <v>25</v>
+      </c>
+      <c r="I3" s="3">
+        <v>25</v>
+      </c>
+      <c r="J3" s="3">
+        <v>25</v>
+      </c>
+      <c r="K3" s="3">
+        <v>25</v>
+      </c>
+      <c r="L3" s="3">
+        <v>25</v>
+      </c>
+      <c r="M3" s="3">
+        <v>25</v>
+      </c>
+      <c r="N3" s="3">
+        <v>25</v>
+      </c>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>9901</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>9901</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2301</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>51</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="3">
+        <v>15</v>
+      </c>
+      <c r="F6" s="3">
+        <v>15</v>
+      </c>
+      <c r="G6" s="3">
+        <v>15</v>
+      </c>
+      <c r="H6" s="3">
+        <v>15</v>
+      </c>
+      <c r="I6" s="3">
+        <v>15</v>
+      </c>
+      <c r="J6" s="3">
+        <v>15</v>
+      </c>
+      <c r="K6" s="3">
+        <v>0</v>
+      </c>
+      <c r="L6" s="3">
+        <v>15</v>
+      </c>
+      <c r="M6" s="3">
+        <v>15</v>
+      </c>
+      <c r="N6" s="3">
+        <v>15</v>
+      </c>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1251</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>60</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="3">
+        <v>10</v>
+      </c>
+      <c r="F7" s="3">
+        <v>10</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0</v>
+      </c>
+      <c r="H7" s="3">
+        <v>10</v>
+      </c>
+      <c r="I7" s="3">
+        <v>10</v>
+      </c>
+      <c r="J7" s="3">
+        <v>10</v>
+      </c>
+      <c r="K7" s="3">
+        <v>10</v>
+      </c>
+      <c r="L7" s="3">
+        <v>10</v>
+      </c>
+      <c r="M7" s="3">
+        <v>0</v>
+      </c>
+      <c r="N7" s="3">
+        <v>10</v>
+      </c>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1251</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0</v>
+      </c>
+      <c r="G8" s="3">
+        <v>10</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0</v>
+      </c>
+      <c r="I8" s="3">
+        <v>0</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0</v>
+      </c>
+      <c r="K8" s="3">
+        <v>0</v>
+      </c>
+      <c r="L8" s="3">
+        <v>0</v>
+      </c>
+      <c r="M8" s="3">
+        <v>10</v>
+      </c>
+      <c r="N8" s="3">
+        <v>0</v>
+      </c>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>1321</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9">
+        <v>60</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="3">
+        <v>5</v>
+      </c>
+      <c r="F9" s="3">
+        <v>5</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0</v>
+      </c>
+      <c r="H9" s="3">
+        <v>5</v>
+      </c>
+      <c r="I9" s="3">
+        <v>5</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0</v>
+      </c>
+      <c r="K9" s="3">
+        <v>0</v>
+      </c>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1321</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10">
+        <v>61</v>
+      </c>
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0</v>
+      </c>
+      <c r="I10" s="3">
+        <v>0</v>
+      </c>
+      <c r="J10" s="3">
+        <v>5</v>
+      </c>
+      <c r="K10" s="3">
+        <v>5</v>
+      </c>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>1321</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11">
+        <v>59</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0</v>
+      </c>
+      <c r="G11" s="3">
+        <v>5</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0</v>
+      </c>
+      <c r="J11" s="3">
+        <v>0</v>
+      </c>
+      <c r="K11" s="3">
+        <v>0</v>
+      </c>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2271</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12">
+        <v>60</v>
+      </c>
+      <c r="D12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="3">
+        <v>5</v>
+      </c>
+      <c r="F12" s="3">
+        <v>5</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0</v>
+      </c>
+      <c r="H12" s="3">
+        <v>0</v>
+      </c>
+      <c r="I12" s="3">
+        <v>0</v>
+      </c>
+      <c r="J12" s="3">
+        <v>0</v>
+      </c>
+      <c r="K12" s="3">
+        <v>0</v>
+      </c>
+      <c r="L12" s="3">
+        <v>5</v>
+      </c>
+      <c r="M12" s="3">
+        <v>0</v>
+      </c>
+      <c r="N12" s="3">
+        <v>0</v>
+      </c>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>2271</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13">
+        <v>59</v>
+      </c>
+      <c r="D13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0</v>
+      </c>
+      <c r="G13" s="3">
+        <v>5</v>
+      </c>
+      <c r="H13" s="3">
+        <v>5</v>
+      </c>
+      <c r="I13" s="3">
+        <v>5</v>
+      </c>
+      <c r="J13" s="3">
+        <v>0</v>
+      </c>
+      <c r="K13" s="3">
+        <v>0</v>
+      </c>
+      <c r="L13" s="3">
+        <v>0</v>
+      </c>
+      <c r="M13" s="3">
+        <v>5</v>
+      </c>
+      <c r="N13" s="3">
+        <v>5</v>
+      </c>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>2271</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14">
+        <v>61</v>
+      </c>
+      <c r="D14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0</v>
+      </c>
+      <c r="G14" s="3">
+        <v>0</v>
+      </c>
+      <c r="H14" s="3">
+        <v>0</v>
+      </c>
+      <c r="I14" s="3">
+        <v>0</v>
+      </c>
+      <c r="J14" s="3">
+        <v>5</v>
+      </c>
+      <c r="K14" s="3">
+        <v>5</v>
+      </c>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="L15" s="2"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="L16" s="2"/>
+      <c r="Q16" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="R16" t="s">
+        <v>26</v>
+      </c>
+      <c r="S16" t="s">
+        <v>27</v>
+      </c>
+      <c r="T16" t="s">
+        <v>28</v>
+      </c>
+      <c r="U16" t="s">
+        <v>30</v>
+      </c>
+      <c r="V16" t="s">
+        <v>31</v>
+      </c>
+      <c r="W16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="12:23" x14ac:dyDescent="0.2">
+      <c r="L17" s="2"/>
+      <c r="Q17" s="5">
+        <v>10</v>
+      </c>
+      <c r="R17" s="6">
+        <v>50</v>
+      </c>
+      <c r="S17" s="6">
+        <v>50</v>
+      </c>
+      <c r="T17" s="6">
+        <v>60</v>
+      </c>
+      <c r="U17" s="6">
+        <v>50</v>
+      </c>
+      <c r="V17" s="6">
+        <v>50</v>
+      </c>
+      <c r="W17" s="6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="12:23" x14ac:dyDescent="0.2">
+      <c r="L18" s="2"/>
+      <c r="Q18" s="5">
         <v>20</v>
       </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="2">
+      <c r="R18" s="6">
+        <v>40</v>
+      </c>
+      <c r="S18" s="6">
+        <v>40</v>
+      </c>
+      <c r="T18" s="6">
+        <v>50</v>
+      </c>
+      <c r="U18" s="6">
+        <v>45</v>
+      </c>
+      <c r="V18" s="6">
+        <v>45</v>
+      </c>
+      <c r="W18" s="6">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="12:23" x14ac:dyDescent="0.2">
+      <c r="L19" s="2"/>
+      <c r="Q19" s="5">
+        <v>60</v>
+      </c>
+      <c r="R19" s="6">
+        <v>20</v>
+      </c>
+      <c r="S19" s="6">
+        <v>20</v>
+      </c>
+      <c r="T19" s="6">
+        <v>0</v>
+      </c>
+      <c r="U19" s="6">
+        <v>15</v>
+      </c>
+      <c r="V19" s="6">
+        <v>15</v>
+      </c>
+      <c r="W19" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="12:23" x14ac:dyDescent="0.2">
+      <c r="L20" s="2"/>
+      <c r="Q20" s="5">
+        <v>61</v>
+      </c>
+      <c r="R20" s="6">
+        <v>0</v>
+      </c>
+      <c r="S20" s="6">
+        <v>0</v>
+      </c>
+      <c r="T20" s="6">
+        <v>0</v>
+      </c>
+      <c r="U20" s="6">
+        <v>0</v>
+      </c>
+      <c r="V20" s="6">
+        <v>0</v>
+      </c>
+      <c r="W20" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="12:23" x14ac:dyDescent="0.2">
+      <c r="L21" s="2"/>
+      <c r="Q21" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="2">
-        <v>25</v>
-      </c>
-      <c r="H3" s="2">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
-      <c r="B4">
-        <v>2301</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4">
-        <v>20</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="2">
-        <v>15</v>
-      </c>
-      <c r="G4" s="2">
-        <v>15</v>
-      </c>
-      <c r="H4" s="2">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
-      <c r="B5">
-        <v>1251</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5">
-        <v>60</v>
-      </c>
-      <c r="E5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="2">
-        <v>10</v>
-      </c>
-      <c r="G5" s="2">
-        <v>0</v>
-      </c>
-      <c r="H5" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
-      <c r="B6">
-        <v>1251</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6">
-        <v>10</v>
-      </c>
-      <c r="E6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0</v>
-      </c>
-      <c r="G6" s="2">
-        <v>10</v>
-      </c>
-      <c r="H6" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="2"/>
-      <c r="B7">
-        <v>2271</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7">
-        <v>60</v>
-      </c>
-      <c r="E7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="2">
-        <v>5</v>
-      </c>
-      <c r="G7" s="2">
-        <v>0</v>
-      </c>
-      <c r="H7" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="2"/>
-      <c r="B8">
-        <v>2271</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8">
-        <v>20</v>
-      </c>
-      <c r="E8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="2">
-        <v>0</v>
-      </c>
-      <c r="G8" s="2">
-        <v>5</v>
-      </c>
-      <c r="H8" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="2"/>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C18" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18">
-        <v>10</v>
-      </c>
-      <c r="E18" t="s">
-        <v>7</v>
-      </c>
-      <c r="F18" s="2">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C19" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19">
-        <v>20</v>
-      </c>
-      <c r="E19" t="s">
-        <v>10</v>
-      </c>
-      <c r="F19" s="2">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C20" t="s">
-        <v>13</v>
-      </c>
-      <c r="D20">
-        <v>20</v>
-      </c>
-      <c r="E20" t="s">
-        <v>9</v>
-      </c>
-      <c r="F20" s="2">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D21">
-        <v>60</v>
-      </c>
-      <c r="E21" t="s">
-        <v>11</v>
-      </c>
-      <c r="F21" s="2">
-        <v>10</v>
-      </c>
-      <c r="G21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C22" t="s">
-        <v>17</v>
-      </c>
-      <c r="D22">
-        <v>20</v>
-      </c>
-      <c r="E22" t="s">
-        <v>15</v>
-      </c>
-      <c r="F22" s="2">
-        <v>5</v>
-      </c>
-      <c r="G22" t="s">
-        <v>21</v>
-      </c>
+      <c r="R21" s="6">
+        <v>110</v>
+      </c>
+      <c r="S21" s="6">
+        <v>110</v>
+      </c>
+      <c r="T21" s="6">
+        <v>110</v>
+      </c>
+      <c r="U21" s="6">
+        <v>110</v>
+      </c>
+      <c r="V21" s="6">
+        <v>110</v>
+      </c>
+      <c r="W21" s="6">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="12:23" x14ac:dyDescent="0.2">
+      <c r="L22" s="2"/>
+    </row>
+    <row r="23" spans="12:23" x14ac:dyDescent="0.2">
+      <c r="L23" s="2"/>
+    </row>
+    <row r="24" spans="12:23" x14ac:dyDescent="0.2">
+      <c r="L24" s="2"/>
+    </row>
+    <row r="25" spans="12:23" x14ac:dyDescent="0.2">
+      <c r="L25" s="2"/>
+    </row>
+    <row r="26" spans="12:23" x14ac:dyDescent="0.2">
+      <c r="L26" s="2"/>
+    </row>
+    <row r="27" spans="12:23" x14ac:dyDescent="0.2">
+      <c r="L27" s="2"/>
+    </row>
+    <row r="28" spans="12:23" x14ac:dyDescent="0.2">
+      <c r="L28" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>